<commit_message>
correcting mtab name error in 2021
</commit_message>
<xml_diff>
--- a/dataFiles/KujLab_metaboliteLookUpTable.xlsx
+++ b/dataFiles/KujLab_metaboliteLookUpTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klongnecker\Documents\Dropbox\Current projects\Kuj_BIOSSCOPE\RawData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klongnecker\Documents\GitHub\BIOSSCOPE_targetedMtabs\dataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4AF4CA-6EE3-4EE9-AB8B-524F3C486B19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52B78FF-3D3D-4895-AF97-43175098EB22}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26670" windowHeight="13350" xr2:uid="{5A1B3757-BF0E-49DB-BC24-9E591F8C7912}"/>
   </bookViews>
@@ -1215,20 +1215,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED613801-DCA0-4263-A3BD-5371038F8D0C}">
   <dimension ref="A1:D256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C148" sqref="C148"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="47.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="47.26953125" style="1" customWidth="1"/>
     <col min="2" max="2" width="37" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="38.5703125" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="9.42578125" style="1"/>
+    <col min="3" max="3" width="41.54296875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="38.54296875" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="9.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>179</v>
       </c>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>209</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>205</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>203</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>182</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>181</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>180</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>214</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>62</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>220</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>183</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>217</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>184</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>223</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>185</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>20</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>21</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>177</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>24</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>27</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>28</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>29</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>30</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>31</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>32</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>33</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>34</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>35</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>71</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="7" t="s">
         <v>186</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>36</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>37</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>3</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>187</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>39</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>40</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>41</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>42</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>43</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>44</v>
       </c>
@@ -2028,7 +2028,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>45</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>46</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>47</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>48</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>49</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>50</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>51</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>54</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>55</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>188</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>23</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>56</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>57</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>58</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>59</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>53</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>61</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>189</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>63</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>64</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" s="7" t="s">
         <v>190</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>65</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
         <v>191</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>66</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>67</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>68</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
         <v>240</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>69</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>70</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>74</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>75</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" s="8" t="s">
         <v>192</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>77</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>78</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>79</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>80</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>81</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>82</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
         <v>193</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>83</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>84</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>85</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>86</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
         <v>194</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>13</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" s="7" t="s">
         <v>195</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>87</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>88</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>94</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>89</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>90</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" s="7" t="s">
         <v>196</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>91</v>
       </c>
@@ -2715,13 +2715,13 @@
         <v>163</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>255</v>
+        <v>163</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>92</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>93</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>38</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>95</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>96</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>97</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>98</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>99</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>100</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>259</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>101</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>178</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>102</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>103</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>105</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>106</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>107</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>108</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>104</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>109</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>110</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>111</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>112</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" s="8" t="s">
         <v>197</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>113</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>114</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>76</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146" s="3" t="s">
         <v>198</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>115</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" s="7" t="s">
         <v>199</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149" s="3" t="s">
         <v>200</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>264</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>116</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>117</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>118</v>
       </c>
@@ -3180,193 +3180,193 @@
         <v>173</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154" s="3"/>
       <c r="B154"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155" s="3"/>
       <c r="B155"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156" s="3"/>
       <c r="B156"/>
     </row>
-    <row r="190" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D190" s="1"/>
     </row>
-    <row r="191" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D191" s="1"/>
     </row>
-    <row r="192" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D192" s="1"/>
     </row>
-    <row r="193" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D193" s="1"/>
     </row>
-    <row r="194" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D194" s="1"/>
     </row>
-    <row r="195" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D195" s="1"/>
     </row>
-    <row r="196" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D196" s="1"/>
     </row>
-    <row r="197" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D197" s="1"/>
     </row>
-    <row r="198" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D198" s="1"/>
     </row>
-    <row r="199" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D199" s="1"/>
     </row>
-    <row r="201" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D201" s="1"/>
     </row>
-    <row r="202" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D202" s="1"/>
     </row>
-    <row r="205" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D205" s="1"/>
     </row>
-    <row r="206" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D206" s="1"/>
     </row>
-    <row r="207" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D207" s="1"/>
     </row>
-    <row r="208" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D208" s="1"/>
     </row>
-    <row r="209" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D209" s="1"/>
     </row>
-    <row r="212" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D212" s="1"/>
     </row>
-    <row r="213" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D213" s="1"/>
     </row>
-    <row r="214" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D214" s="1"/>
     </row>
-    <row r="215" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D215" s="1"/>
     </row>
-    <row r="216" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D216" s="1"/>
     </row>
-    <row r="217" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D217" s="1"/>
     </row>
-    <row r="218" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D218" s="1"/>
     </row>
-    <row r="219" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D219" s="1"/>
     </row>
-    <row r="220" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D220" s="1"/>
     </row>
-    <row r="221" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D221" s="1"/>
     </row>
-    <row r="222" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D222" s="1"/>
     </row>
-    <row r="223" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D223" s="1"/>
     </row>
-    <row r="224" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D224" s="1"/>
     </row>
-    <row r="226" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D226" s="1"/>
     </row>
-    <row r="227" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D227" s="1"/>
     </row>
-    <row r="228" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D228" s="1"/>
     </row>
-    <row r="229" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D229" s="1"/>
     </row>
-    <row r="230" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D230" s="1"/>
     </row>
-    <row r="231" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D231" s="1"/>
     </row>
-    <row r="232" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D232" s="1"/>
     </row>
-    <row r="233" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D233" s="1"/>
     </row>
-    <row r="234" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D234" s="1"/>
     </row>
-    <row r="235" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D235" s="1"/>
     </row>
-    <row r="236" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D236" s="1"/>
     </row>
-    <row r="237" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D237" s="1"/>
     </row>
-    <row r="238" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D238" s="1"/>
     </row>
-    <row r="239" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D239" s="1"/>
     </row>
-    <row r="240" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D240" s="1"/>
     </row>
-    <row r="241" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D241" s="1"/>
     </row>
-    <row r="242" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D242" s="1"/>
     </row>
-    <row r="243" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D243" s="1"/>
     </row>
-    <row r="244" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D244" s="1"/>
     </row>
-    <row r="245" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D245" s="1"/>
     </row>
-    <row r="247" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D247" s="1"/>
     </row>
-    <row r="248" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D248" s="1"/>
     </row>
-    <row r="250" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D250" s="1"/>
     </row>
-    <row r="251" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D251" s="1"/>
     </row>
-    <row r="252" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D252" s="1"/>
     </row>
-    <row r="253" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D253" s="1"/>
     </row>
-    <row r="254" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="254" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D254" s="1"/>
     </row>
-    <row r="255" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="255" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D255" s="1"/>
     </row>
-    <row r="256" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="256" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D256" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correcting two isomers KL had backwards
</commit_message>
<xml_diff>
--- a/dataFiles/KujLab_metaboliteLookUpTable.xlsx
+++ b/dataFiles/KujLab_metaboliteLookUpTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klongnecker\Documents\GitHub\BIOSSCOPE_targetedMtabs\dataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klongnecker\Documents\Dropbox\GitHub\BIOSSCOPE_targetedMtabs\dataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA8C18B-22EB-4DAF-9CC8-E3112604898D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EAA72D2-E9BA-471B-8CEC-FE757A61AB62}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26670" windowHeight="13350" xr2:uid="{5A1B3757-BF0E-49DB-BC24-9E591F8C7912}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="266">
   <si>
     <t>cleanName</t>
   </si>
@@ -558,12 +558,6 @@
     <t>SRMname_2023</t>
   </si>
   <si>
-    <t>beta-alanine (isom. alanine)</t>
-  </si>
-  <si>
-    <t>sarcosine</t>
-  </si>
-  <si>
     <t>(6R)-5-6-7-8-tetrahydrobiopterin</t>
   </si>
   <si>
@@ -826,6 +820,9 @@
   </si>
   <si>
     <t>uridine neg</t>
+  </si>
+  <si>
+    <t>beta-alanine</t>
   </si>
 </sst>
 </file>
@@ -1199,22 +1196,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED613801-DCA0-4263-A3BD-5371038F8D0C}">
-  <dimension ref="A1:D256"/>
+  <dimension ref="A1:D255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="C118" sqref="C118"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="D130" sqref="D130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.26953125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="47.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="37" style="2" customWidth="1"/>
-    <col min="3" max="3" width="41.54296875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="38.54296875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="9.453125" style="2"/>
+    <col min="3" max="3" width="41.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="9.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1228,18 +1225,18 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>123</v>
@@ -1248,10 +1245,10 @@
         <v>123</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1262,10 +1259,10 @@
         <v>119</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -1273,24 +1270,24 @@
         <v>120</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>121</v>
@@ -1299,40 +1296,40 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
@@ -1343,9 +1340,9 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>125</v>
@@ -1354,7 +1351,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
@@ -1365,7 +1362,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>6</v>
       </c>
@@ -1373,10 +1370,10 @@
         <v>126</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
@@ -1390,7 +1387,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>8</v>
       </c>
@@ -1404,7 +1401,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>62</v>
       </c>
@@ -1418,7 +1415,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1432,7 +1429,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>9</v>
       </c>
@@ -1446,7 +1443,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>10</v>
       </c>
@@ -1460,7 +1457,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>11</v>
       </c>
@@ -1474,7 +1471,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>60</v>
       </c>
@@ -1488,50 +1485,50 @@
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
+      <c r="C25" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>12</v>
       </c>
@@ -1545,7 +1542,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>14</v>
       </c>
@@ -1553,13 +1550,13 @@
         <v>129</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>15</v>
       </c>
@@ -1570,24 +1567,24 @@
         <v>15</v>
       </c>
       <c r="D29" s="4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>225</v>
-      </c>
       <c r="D30" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>16</v>
       </c>
@@ -1597,8 +1594,11 @@
       <c r="C31" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D31" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>17</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>52</v>
       </c>
@@ -1626,19 +1626,19 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>19</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>20</v>
       </c>
@@ -1663,10 +1663,10 @@
         <v>131</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>21</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>22</v>
       </c>
@@ -1685,22 +1685,22 @@
         <v>132</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>177</v>
+        <v>265</v>
       </c>
       <c r="B39" s="5"/>
       <c r="D39" s="4" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>24</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>25</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>26</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>27</v>
       </c>
@@ -1747,10 +1747,10 @@
         <v>135</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>28</v>
       </c>
@@ -1761,10 +1761,10 @@
         <v>28</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>29</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>30</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>31</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>32</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>33</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>34</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>35</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>71</v>
       </c>
@@ -1873,16 +1873,16 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B53" s="5"/>
       <c r="D53" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>36</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>37</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>3</v>
       </c>
@@ -1921,19 +1921,19 @@
         <v>122</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>39</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>40</v>
       </c>
@@ -1955,10 +1955,10 @@
         <v>139</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>41</v>
       </c>
@@ -1969,10 +1969,10 @@
         <v>41</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>42</v>
       </c>
@@ -1983,10 +1983,10 @@
         <v>42</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>43</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>44</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>45</v>
       </c>
@@ -2025,10 +2025,10 @@
         <v>45</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>46</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>47</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>48</v>
       </c>
@@ -2064,13 +2064,13 @@
         <v>142</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>49</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>50</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>51</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>54</v>
       </c>
@@ -2120,10 +2120,10 @@
         <v>54</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>55</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>72</v>
       </c>
@@ -2145,10 +2145,10 @@
         <v>72</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>73</v>
       </c>
@@ -2156,22 +2156,22 @@
         <v>152</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B75" s="5"/>
       <c r="D75" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>23</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>56</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>57</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>58</v>
       </c>
@@ -2215,13 +2215,13 @@
         <v>145</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>59</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>53</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>61</v>
       </c>
@@ -2260,19 +2260,19 @@
         <v>61</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>63</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>64</v>
       </c>
@@ -2300,16 +2300,16 @@
         <v>64</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B86" s="5"/>
       <c r="D86" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>65</v>
       </c>
@@ -2323,16 +2323,16 @@
         <v>65</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B88" s="5"/>
       <c r="C88" s="4" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>66</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>67</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>68</v>
       </c>
@@ -2371,19 +2371,19 @@
         <v>68</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B92" s="5"/>
       <c r="C92" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>69</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>70</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>74</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>75</v>
       </c>
@@ -2439,16 +2439,16 @@
         <v>75</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B97" s="5"/>
       <c r="D97" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>77</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>78</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>79</v>
       </c>
@@ -2484,10 +2484,10 @@
         <v>156</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>80</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>81</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>82</v>
       </c>
@@ -2520,16 +2520,16 @@
         <v>82</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B104" s="5"/>
       <c r="C104" s="4" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>83</v>
       </c>
@@ -2540,10 +2540,10 @@
         <v>158</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>84</v>
       </c>
@@ -2554,10 +2554,10 @@
         <v>84</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>85</v>
       </c>
@@ -2565,13 +2565,13 @@
         <v>159</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>86</v>
       </c>
@@ -2582,22 +2582,22 @@
         <v>160</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B109" s="5"/>
       <c r="C109" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>13</v>
       </c>
@@ -2611,16 +2611,16 @@
         <v>128</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B111" s="5"/>
       <c r="D111" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>87</v>
       </c>
@@ -2631,10 +2631,10 @@
         <v>161</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>88</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>94</v>
       </c>
@@ -2650,13 +2650,13 @@
         <v>164</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>89</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>90</v>
       </c>
@@ -2684,16 +2684,16 @@
         <v>90</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B117" s="5"/>
       <c r="D117" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>91</v>
       </c>
@@ -2704,10 +2704,10 @@
         <v>163</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>92</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>93</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>38</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>95</v>
       </c>
@@ -2757,13 +2757,13 @@
         <v>165</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>96</v>
       </c>
@@ -2774,7 +2774,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>97</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>98</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>99</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>100</v>
       </c>
@@ -2830,21 +2830,21 @@
         <v>100</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>101</v>
       </c>
@@ -2855,506 +2855,497 @@
         <v>166</v>
       </c>
       <c r="D129" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D131" s="4" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A130" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="B130" s="5"/>
-      <c r="D130" s="4" t="s">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C132" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D132" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C133" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D133" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D134" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D136" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B137" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C137" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D137" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D138" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D139" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D140" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B141" s="5"/>
+      <c r="D141" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B142" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B143" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C143" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D143" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B144" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C144" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D144" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B145" s="5"/>
+      <c r="D145" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C146" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D146" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B147" s="5"/>
+      <c r="D147" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B148" s="5"/>
+      <c r="C148" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="D148" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="5" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A131" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B131" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C131" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D131" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A132" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B132" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C132" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="D132" s="4" t="s">
+      <c r="B149" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D149" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B150" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C150" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D150" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B151" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C151" s="4" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A133" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B133" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C133" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D133" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A134" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B134" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C134" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D134" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A135" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B135" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C135" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D135" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A136" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B136" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C136" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D136" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A137" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B137" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C137" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="D137" s="4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A138" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B138" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C138" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D138" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A139" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B139" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C139" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D139" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A140" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B140" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="C140" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D140" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A141" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B141" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C141" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D141" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A142" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="B142" s="5"/>
-      <c r="D142" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A143" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B143" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A144" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B144" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C144" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D144" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A145" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B145" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C145" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D145" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A146" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B146" s="5"/>
-      <c r="D146" s="4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A147" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B147" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C147" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="D147" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A148" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B148" s="5"/>
-      <c r="D148" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A149" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B149" s="5"/>
-      <c r="C149" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="D149" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A150" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="B150" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="C150" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="D150" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A151" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B151" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C151" s="4" t="s">
-        <v>116</v>
-      </c>
       <c r="D151" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>265</v>
+        <v>173</v>
       </c>
       <c r="D152" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A153" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B153" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="C153" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D153" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B153" s="5"/>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B154" s="5"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B155" s="5"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B156" s="5"/>
-    </row>
-    <row r="190" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="189" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D189" s="2"/>
+    </row>
+    <row r="190" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D190" s="2"/>
     </row>
-    <row r="191" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="191" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D191" s="2"/>
     </row>
-    <row r="192" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="192" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D192" s="2"/>
     </row>
-    <row r="193" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="193" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D193" s="2"/>
     </row>
-    <row r="194" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="194" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D194" s="2"/>
     </row>
-    <row r="195" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="195" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D195" s="2"/>
     </row>
-    <row r="196" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="196" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D196" s="2"/>
     </row>
-    <row r="197" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="197" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D197" s="2"/>
     </row>
-    <row r="198" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="198" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D198" s="2"/>
     </row>
-    <row r="199" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D199" s="2"/>
-    </row>
-    <row r="201" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="200" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D200" s="2"/>
+    </row>
+    <row r="201" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D201" s="2"/>
     </row>
-    <row r="202" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D202" s="2"/>
-    </row>
-    <row r="205" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="204" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D204" s="2"/>
+    </row>
+    <row r="205" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D205" s="2"/>
     </row>
-    <row r="206" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="206" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D206" s="2"/>
     </row>
-    <row r="207" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="207" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D207" s="2"/>
     </row>
-    <row r="208" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="208" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D208" s="2"/>
     </row>
-    <row r="209" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D209" s="2"/>
-    </row>
-    <row r="212" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="211" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D211" s="2"/>
+    </row>
+    <row r="212" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D212" s="2"/>
     </row>
-    <row r="213" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="213" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D213" s="2"/>
     </row>
-    <row r="214" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="214" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D214" s="2"/>
     </row>
-    <row r="215" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="215" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D215" s="2"/>
     </row>
-    <row r="216" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="216" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D216" s="2"/>
     </row>
-    <row r="217" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="217" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D217" s="2"/>
     </row>
-    <row r="218" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="218" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D218" s="2"/>
     </row>
-    <row r="219" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="219" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D219" s="2"/>
     </row>
-    <row r="220" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="220" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D220" s="2"/>
     </row>
-    <row r="221" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="221" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D221" s="2"/>
     </row>
-    <row r="222" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="222" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D222" s="2"/>
     </row>
-    <row r="223" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="223" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D223" s="2"/>
     </row>
-    <row r="224" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D224" s="2"/>
-    </row>
-    <row r="226" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="225" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D225" s="2"/>
+    </row>
+    <row r="226" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D226" s="2"/>
     </row>
-    <row r="227" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="227" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D227" s="2"/>
     </row>
-    <row r="228" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="228" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D228" s="2"/>
     </row>
-    <row r="229" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="229" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D229" s="2"/>
     </row>
-    <row r="230" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="230" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D230" s="2"/>
     </row>
-    <row r="231" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="231" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D231" s="2"/>
     </row>
-    <row r="232" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="232" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D232" s="2"/>
     </row>
-    <row r="233" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="233" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D233" s="2"/>
     </row>
-    <row r="234" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="234" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D234" s="2"/>
     </row>
-    <row r="235" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="235" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D235" s="2"/>
     </row>
-    <row r="236" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="236" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D236" s="2"/>
     </row>
-    <row r="237" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="237" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D237" s="2"/>
     </row>
-    <row r="238" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="238" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D238" s="2"/>
     </row>
-    <row r="239" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="239" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D239" s="2"/>
     </row>
-    <row r="240" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="240" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D240" s="2"/>
     </row>
-    <row r="241" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="241" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D241" s="2"/>
     </row>
-    <row r="242" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="242" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D242" s="2"/>
     </row>
-    <row r="243" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="243" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D243" s="2"/>
     </row>
-    <row r="244" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="244" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D244" s="2"/>
     </row>
-    <row r="245" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D245" s="2"/>
-    </row>
-    <row r="247" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="246" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D246" s="2"/>
+    </row>
+    <row r="247" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D247" s="2"/>
     </row>
-    <row r="248" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D248" s="2"/>
-    </row>
-    <row r="250" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="249" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D249" s="2"/>
+    </row>
+    <row r="250" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D250" s="2"/>
     </row>
-    <row r="251" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="251" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D251" s="2"/>
     </row>
-    <row r="252" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="252" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D252" s="2"/>
     </row>
-    <row r="253" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="253" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D253" s="2"/>
     </row>
-    <row r="254" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="254" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D254" s="2"/>
     </row>
-    <row r="255" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="255" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D255" s="2"/>
     </row>
-    <row r="256" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D256" s="2"/>
-    </row>
   </sheetData>
-  <sortState ref="A2:G258">
-    <sortCondition ref="A2:A258"/>
+  <sortState ref="A2:G257">
+    <sortCondition ref="A2:A257"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>